<commit_message>
added more test coverage and made some changes to methods
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestDataShareSkill.xlsx
+++ b/MarsFramework/ExcelData/TestDataShareSkill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c6460faf6f83a1b/Documents/Mars Competition Task-2/MarsFramework/ExcelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{2AB6CD75-D27A-4461-9128-068236250026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4553140-E5A9-4F96-8880-6D0829E49E6E}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{2AB6CD75-D27A-4461-9128-068236250026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2EF58D1-43C8-4574-9F06-F76B2A82985D}"/>
   <bookViews>
-    <workbookView xWindow="-5565" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="67">
   <si>
     <t>Url</t>
   </si>
@@ -211,6 +211,33 @@
   </si>
   <si>
     <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>Digital Marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advertising </t>
+  </si>
+  <si>
+    <t>Design website banners and assist with web visuals</t>
+  </si>
+  <si>
+    <t>Social Media Marketing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Testtesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttesttestt105</t>
+  </si>
+  <si>
+    <t>Testtesttesttestte20</t>
+  </si>
+  <si>
+    <t>Testing Software and Web ApplicationsTesting 555 Testing Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web Applications403Testing Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web Ap600603</t>
+  </si>
+  <si>
+    <t>Testing Software and Web ApplicationsTesting 555 Testing Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web ApplicationsTesting Software and Web Applications197</t>
   </si>
 </sst>
 </file>
@@ -220,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +267,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -272,7 +305,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -281,6 +314,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -729,10 +765,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -740,7 +776,7 @@
     <col min="1" max="1" width="20.109375" customWidth="1"/>
     <col min="2" max="2" width="48.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.88671875" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.88671875" customWidth="1"/>
     <col min="6" max="6" width="24.88671875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
@@ -898,6 +934,78 @@
       </c>
       <c r="P3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1038,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD7A40F-0C5C-4B03-B919-DF0C16BB76A2}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>